<commit_message>
Estadisticos Segundo Parcial 23 Mayo
</commit_message>
<xml_diff>
--- a/Totales Generales20242.xlsx
+++ b/Totales Generales20242.xlsx
@@ -629,10 +629,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -685,34 +685,34 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>7</v>
       </c>
       <c r="L3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M3">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="N3">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="O3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="P3" s="1">
-        <v>47.1</v>
+        <v>31.4</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -779,40 +779,40 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
       <c r="I5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K5">
         <v>30</v>
       </c>
       <c r="L5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="N5">
-        <v>391</v>
+        <v>421</v>
       </c>
       <c r="O5">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="P5" s="1">
-        <v>38.4</v>
+        <v>33.7</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -826,34 +826,34 @@
         <v>128</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
       <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6">
         <v>10</v>
       </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>17</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
-      </c>
       <c r="M6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N6">
         <v>39</v>
@@ -879,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -900,19 +900,19 @@
         <v>9</v>
       </c>
       <c r="L7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7">
         <v>18</v>
       </c>
       <c r="N7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P7" s="1">
-        <v>62.7</v>
+        <v>61.4</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -976,43 +976,43 @@
         <v>326</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
       <c r="H9">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K9">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L9">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M9">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N9">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O9">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P9" s="1">
-        <v>56.4</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1023,43 +1023,43 @@
         <v>961</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J10">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K10">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L10">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M10">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="N10">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="O10">
-        <v>428</v>
+        <v>397</v>
       </c>
       <c r="P10" s="1">
-        <v>44.5</v>
+        <v>41.3</v>
       </c>
     </row>
   </sheetData>
@@ -1139,43 +1139,43 @@
         <v>234</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="O2">
-        <v>234</v>
+        <v>99</v>
       </c>
       <c r="P2" s="1">
-        <v>100</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1192,31 +1192,31 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1251,31 +1251,31 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="O4">
-        <v>210</v>
+        <v>47</v>
       </c>
       <c r="P4" s="1">
-        <v>100</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1289,43 +1289,43 @@
         <v>635</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>321</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="O5">
-        <v>635</v>
+        <v>337</v>
       </c>
       <c r="P5" s="1">
-        <v>100</v>
+        <v>53.1</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1339,34 +1339,34 @@
         <v>128</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1392,40 +1392,40 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O7">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="P7" s="1">
-        <v>100</v>
+        <v>72.3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1451,31 +1451,31 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="O8">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="P8" s="1">
-        <v>100</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1489,43 +1489,43 @@
         <v>326</v>
       </c>
       <c r="D9">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="L9">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="O9">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="P9" s="1">
-        <v>100</v>
+        <v>84.40000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1536,43 +1536,43 @@
         <v>961</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>26</v>
+      </c>
+      <c r="J10">
+        <v>39</v>
+      </c>
+      <c r="K10">
         <v>54</v>
       </c>
-      <c r="E10">
-        <v>468</v>
-      </c>
-      <c r="F10">
-        <v>110</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>324</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
       <c r="L10">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>349</v>
       </c>
       <c r="O10">
-        <v>961</v>
+        <v>612</v>
       </c>
       <c r="P10" s="1">
-        <v>100</v>
+        <v>63.7</v>
       </c>
     </row>
   </sheetData>
@@ -1652,43 +1652,43 @@
         <v>234</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J2">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="L2">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="M2">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="O2">
-        <v>234</v>
+        <v>67</v>
       </c>
       <c r="P2" s="1">
-        <v>100</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1708,37 +1708,37 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="L3">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="M3">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="O3">
-        <v>191</v>
+        <v>32</v>
       </c>
       <c r="P3" s="1">
-        <v>100</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1764,31 +1764,31 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M4">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="N4">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="O4">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P4" s="1">
-        <v>19.5</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1802,43 +1802,43 @@
         <v>635</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J5">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K5">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="L5">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="M5">
-        <v>244</v>
+        <v>54</v>
       </c>
       <c r="N5">
-        <v>169</v>
+        <v>499</v>
       </c>
       <c r="O5">
-        <v>466</v>
+        <v>136</v>
       </c>
       <c r="P5" s="1">
-        <v>73.40000000000001</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1852,43 +1852,43 @@
         <v>128</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
       <c r="H6">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I6">
         <v>7</v>
       </c>
       <c r="J6">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K6">
+        <v>22</v>
+      </c>
+      <c r="L6">
         <v>11</v>
       </c>
-      <c r="L6">
-        <v>18</v>
-      </c>
       <c r="M6">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="O6">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="P6" s="1">
-        <v>100</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1905,40 +1905,40 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L7">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="M7">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="O7">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="P7" s="1">
-        <v>97.59999999999999</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1967,28 +1967,28 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
         <v>5</v>
       </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
+      <c r="M8">
         <v>10</v>
       </c>
-      <c r="L8">
-        <v>8</v>
-      </c>
-      <c r="M8">
-        <v>15</v>
-      </c>
       <c r="N8">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="O8">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="P8" s="1">
-        <v>37.4</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2002,43 +2002,43 @@
         <v>326</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="G9">
-        <v>15</v>
-      </c>
       <c r="H9">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J9">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="K9">
         <v>36</v>
       </c>
       <c r="L9">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="M9">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="N9">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="O9">
-        <v>252</v>
+        <v>144</v>
       </c>
       <c r="P9" s="1">
-        <v>77.3</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2049,43 +2049,43 @@
         <v>961</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="I10">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="J10">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="K10">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="L10">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="M10">
-        <v>328</v>
+        <v>100</v>
       </c>
       <c r="N10">
-        <v>243</v>
+        <v>681</v>
       </c>
       <c r="O10">
-        <v>718</v>
+        <v>280</v>
       </c>
       <c r="P10" s="1">
-        <v>74.7</v>
+        <v>29.1</v>
       </c>
     </row>
   </sheetData>
@@ -2165,16 +2165,16 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -2183,19 +2183,19 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L2">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N2">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="O2" s="1">
-        <v>100</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2221,28 +2221,28 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="N3">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1">
-        <v>100</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2253,43 +2253,43 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>3</v>
       </c>
-      <c r="K4">
-        <v>7</v>
-      </c>
-      <c r="L4">
-        <v>13</v>
-      </c>
       <c r="M4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N4">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="O4" s="1">
-        <v>100</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2303,40 +2303,40 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
       <c r="L5">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N5">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="O5" s="1">
-        <v>100</v>
+        <v>34.7</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2356,34 +2356,34 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
         <v>9</v>
       </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
-      </c>
       <c r="M6">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N6">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="O6" s="1">
-        <v>100</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2406,31 +2406,31 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="N7">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="O7" s="1">
-        <v>100</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2456,28 +2456,28 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>17</v>
+      </c>
+      <c r="N8">
         <v>7</v>
       </c>
-      <c r="L8">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>24</v>
-      </c>
       <c r="O8" s="1">
-        <v>100</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2506,25 +2506,25 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N9">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="O9" s="1">
-        <v>100</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -2544,34 +2544,34 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
         <v>27</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
       <c r="N10">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="O10" s="1">
-        <v>100</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2597,28 +2597,28 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N11">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="O11" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -2641,31 +2641,31 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N12">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="O12" s="1">
-        <v>100</v>
+        <v>41.7</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2688,31 +2688,31 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="N13">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="O13" s="1">
-        <v>100</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2750,7 +2750,7 @@
         <v>2</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <v>22</v>
@@ -2788,25 +2788,25 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>37</v>
+      </c>
+      <c r="N15">
         <v>4</v>
       </c>
-      <c r="M15">
-        <v>36</v>
-      </c>
-      <c r="N15">
-        <v>5</v>
-      </c>
       <c r="O15" s="1">
-        <v>12.2</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2835,13 +2835,13 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>4</v>
@@ -2876,31 +2876,31 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M17">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O17" s="1">
-        <v>20.5</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -2929,25 +2929,25 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>4</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N18">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O18" s="1">
-        <v>45.2</v>
+        <v>41.9</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -2985,16 +2985,16 @@
         <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" s="1">
-        <v>5.6</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -3011,37 +3011,37 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K20">
         <v>4</v>
       </c>
       <c r="L20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N20">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="O20" s="1">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -3055,16 +3055,16 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -3079,16 +3079,16 @@
         <v>4</v>
       </c>
       <c r="L21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N21">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="O21" s="1">
-        <v>100</v>
+        <v>60.7</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3099,43 +3099,43 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>2</v>
       </c>
       <c r="K22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
         <v>9</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
       <c r="N22">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="O22" s="1">
-        <v>100</v>
+        <v>60.9</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3152,37 +3152,37 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N23">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="O23" s="1">
-        <v>100</v>
+        <v>46.7</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -3202,34 +3202,34 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N24">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="O24" s="1">
-        <v>100</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -3243,40 +3243,40 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
         <v>3</v>
       </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
       <c r="L25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N25">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="O25" s="1">
-        <v>100</v>
+        <v>68.40000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -3293,37 +3293,37 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
         <v>3</v>
       </c>
-      <c r="J26">
-        <v>4</v>
-      </c>
-      <c r="K26">
-        <v>4</v>
-      </c>
       <c r="L26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N26">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="O26" s="1">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -3343,34 +3343,34 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <v>3</v>
       </c>
       <c r="L27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N27">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O27" s="1">
-        <v>100</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -3399,25 +3399,25 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L28">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N28">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="O28" s="1">
-        <v>93.3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -3449,22 +3449,22 @@
         <v>0</v>
       </c>
       <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
         <v>3</v>
       </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>6</v>
-      </c>
       <c r="M29">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N29">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O29" s="1">
-        <v>90.90000000000001</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -3490,28 +3490,28 @@
         <v>0</v>
       </c>
       <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
         <v>4</v>
       </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>6</v>
-      </c>
       <c r="K30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N30">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O30" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -3537,28 +3537,28 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>3</v>
       </c>
       <c r="K31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M31">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="N31">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O31" s="1">
-        <v>39.3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -3587,25 +3587,25 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>14</v>
+      </c>
+      <c r="N32">
         <v>3</v>
       </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <v>12</v>
-      </c>
-      <c r="N32">
-        <v>5</v>
-      </c>
       <c r="O32" s="1">
-        <v>29.4</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -3640,19 +3640,19 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L33">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M33">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33" s="1">
         <v>8</v>
-      </c>
-      <c r="O33" s="1">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -3681,25 +3681,25 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O34" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3755,19 +3755,19 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>54.1</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>67.59999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3781,19 +3781,19 @@
         <v>29</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1">
         <v>74.40000000000001</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>87.2</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>87.2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3807,19 +3807,19 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1">
         <v>40.6</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3836,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1">
         <v>46.9</v>
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3859,19 +3859,19 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1">
         <v>30.8</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>64.09999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3885,19 +3885,19 @@
         <v>24</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1">
         <v>63.2</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>76.3</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>76.3</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
         <v>29.2</v>
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3934,22 +3934,22 @@
         <v>34</v>
       </c>
       <c r="C9">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1">
-        <v>85.3</v>
+        <v>88.2</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>88.2</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3966,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1">
         <v>87.09999999999999</v>
@@ -3975,7 +3975,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>87.09999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3986,22 +3986,22 @@
         <v>40</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>72.5</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>25</v>
@@ -4027,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>58.3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4044,7 +4044,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1">
         <v>84.2</v>
@@ -4053,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>86.8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4067,7 +4067,7 @@
         <v>22</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>22</v>
@@ -4076,7 +4076,7 @@
         <v>78.59999999999999</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H14" s="1">
         <v>78.59999999999999</v>
@@ -4093,19 +4093,19 @@
         <v>36</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1">
         <v>87.8</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>90.2</v>
       </c>
       <c r="H15" s="1">
-        <v>87.8</v>
+        <v>90.2</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -4119,7 +4119,7 @@
         <v>29</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E16">
         <v>29</v>
@@ -4128,7 +4128,7 @@
         <v>82.90000000000001</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="H16" s="1">
         <v>82.90000000000001</v>
@@ -4145,19 +4145,19 @@
         <v>31</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E17">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1">
         <v>79.5</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>56.4</v>
       </c>
       <c r="H17" s="1">
-        <v>79.5</v>
+        <v>82.09999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -4171,19 +4171,19 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1">
         <v>54.8</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
+        <v>58.1</v>
       </c>
       <c r="H18" s="1">
-        <v>54.8</v>
+        <v>58.1</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -4197,19 +4197,19 @@
         <v>34</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E19">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="1">
         <v>94.40000000000001</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>97.2</v>
       </c>
       <c r="H19" s="1">
-        <v>94.40000000000001</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -4226,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1">
         <v>16.7</v>
@@ -4235,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4252,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1">
         <v>35.7</v>
@@ -4261,7 +4261,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>39.3</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4278,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F22" s="1">
         <v>39.1</v>
@@ -4287,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>39.1</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -4304,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F23" s="1">
         <v>26.7</v>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>53.3</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4330,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F24" s="1">
         <v>54.5</v>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -4353,19 +4353,19 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1">
         <v>10.5</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>31.6</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -4379,19 +4379,19 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1">
         <v>40</v>
       </c>
       <c r="G26" s="1">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4405,19 +4405,19 @@
         <v>4</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1">
         <v>30.8</v>
       </c>
       <c r="G27" s="1">
-        <v>0</v>
+        <v>38.5</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4428,22 +4428,22 @@
         <v>15</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1">
-        <v>53.3</v>
+        <v>60</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>6.7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -4460,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F29" s="1">
         <v>63.6</v>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>9.1</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -4483,19 +4483,19 @@
         <v>5</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1">
         <v>25</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H30" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -4509,19 +4509,19 @@
         <v>17</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E31">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F31" s="1">
         <v>60.7</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H31" s="1">
-        <v>60.7</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -4538,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F32" s="1">
         <v>70.59999999999999</v>
@@ -4547,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <v>70.59999999999999</v>
+        <v>82.40000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -4564,7 +4564,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F33" s="1">
         <v>68</v>
@@ -4573,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F34" s="1">
         <v>84</v>
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="1">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>